<commit_message>
Updated references and dbTables spreadsheet
I finished off 2 references and deleted the cart table from the spreadsheet
</commit_message>
<xml_diff>
--- a/database/dbTables.xlsx
+++ b/database/dbTables.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\h2go\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363E950B-AC88-4CD6-BD3A-C056E2C199D0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043A2BC8-0D6E-4AF6-A33D-45C63732B132}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10630" activeTab="1" xr2:uid="{59BC30C6-78B2-44E3-97A8-010E7BBE7190}"/>
   </bookViews>
   <sheets>
-    <sheet name="cart" sheetId="6" r:id="rId1"/>
-    <sheet name="products" sheetId="1" r:id="rId2"/>
-    <sheet name="users" sheetId="5" r:id="rId3"/>
+    <sheet name="products" sheetId="1" r:id="rId1"/>
+    <sheet name="users" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>Field Name</t>
   </si>
@@ -62,21 +61,9 @@
     <t>productName</t>
   </si>
   <si>
-    <t>fk</t>
-  </si>
-  <si>
-    <t>productType</t>
-  </si>
-  <si>
-    <t>productSize</t>
-  </si>
-  <si>
     <t>blank</t>
   </si>
   <si>
-    <t>productDescription</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
@@ -86,21 +73,9 @@
     <t>float</t>
   </si>
   <si>
-    <t>productInStock</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
     <t>userID</t>
   </si>
   <si>
-    <t>productQuantity</t>
-  </si>
-  <si>
-    <t>totalPrice</t>
-  </si>
-  <si>
     <t>timeStamp</t>
   </si>
   <si>
@@ -131,10 +106,10 @@
     <t>products</t>
   </si>
   <si>
-    <t>cart</t>
-  </si>
-  <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>images</t>
   </si>
 </sst>
 </file>
@@ -504,11 +479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6EC1DC-4F21-469A-9381-E45BE4C35C83}">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CEEC57-4B88-48BE-A2AD-8175ED072FC9}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -524,7 +499,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -559,13 +534,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>255</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -575,16 +556,17 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>255</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -594,18 +576,14 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5">
-        <v>255</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -615,29 +593,21 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3"/>
+      <c r="D6">
+        <v>100</v>
+      </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="E9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -649,11 +619,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CEEC57-4B88-48BE-A2AD-8175ED072FC9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0BB241-EA2D-4A62-861E-5A2C3EFB3625}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -669,7 +639,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -704,10 +674,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>255</v>
@@ -726,17 +696,17 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3">
         <v>255</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -746,17 +716,18 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D5">
         <v>255</v>
       </c>
+      <c r="E5" s="3"/>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -766,17 +737,18 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>255</v>
-      </c>
+        <v>65535</v>
+      </c>
+      <c r="E6" s="3"/>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -786,17 +758,18 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D7">
-        <v>65535</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -806,14 +779,18 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>255</v>
+      </c>
+      <c r="E8" s="3"/>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -823,222 +800,18 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0BB241-EA2D-4A62-861E-5A2C3EFB3625}">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" customWidth="1"/>
-    <col min="3" max="3" width="24.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="32.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>255</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="3">
-        <v>255</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5">
-        <v>255</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6">
-        <v>65535</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7">
-        <v>255</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8">
-        <v>255</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D9">
         <v>255</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Edited database log and dbTables
I don't remember what I did in the spreadsheet in all honesty, and I copy/pasted the database log into the file that I had in the repository instead of keeping it outside it and emailing it. I decided that you guys can just pull everything from here instead of me emailing. Will add the database tomorrow and finalise everything else, but I believe that I have finished.
</commit_message>
<xml_diff>
--- a/database/dbTables.xlsx
+++ b/database/dbTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\h2go\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043A2BC8-0D6E-4AF6-A33D-45C63732B132}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5916F46C-B282-42B8-B453-8BF56E83A5E2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10630" activeTab="1" xr2:uid="{59BC30C6-78B2-44E3-97A8-010E7BBE7190}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10630" xr2:uid="{59BC30C6-78B2-44E3-97A8-010E7BBE7190}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CEEC57-4B88-48BE-A2AD-8175ED072FC9}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0BB241-EA2D-4A62-861E-5A2C3EFB3625}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>